<commit_message>
made some changes to sync 2nd projectleader from central to werkbestand
</commit_message>
<xml_diff>
--- a/Projectleiders.xlsx
+++ b/Projectleiders.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bram.gerrits\Desktop\Automations\ProjectAdministration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9EA1CE-517F-4211-8C0E-3F5F04727DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9218353-74A2-42C3-9963-F023FED81023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
   <si>
     <t>Naam</t>
   </si>
@@ -165,9 +165,6 @@
     <t>TRUE</t>
   </si>
   <si>
-    <t>egbert-jan.holleman@vhe.nl</t>
-  </si>
-  <si>
     <t>dirk.janssen@vhe.nl</t>
   </si>
   <si>
@@ -190,6 +187,12 @@
   </si>
   <si>
     <t>Judith.SetzvanAsten@vhe.nl</t>
+  </si>
+  <si>
+    <t>David Fontijn</t>
+  </si>
+  <si>
+    <t>David.fontijn@vhe.nl</t>
   </si>
 </sst>
 </file>
@@ -520,14 +523,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -549,10 +553,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -565,134 +566,138 @@
         <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D6" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D7" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>20</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" t="s">
-        <v>4</v>
+        <v>21</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>6</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>9</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B18" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -700,7 +705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -708,12 +713,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -721,15 +726,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+      <c r="D26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -737,12 +745,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -750,17 +758,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -789,7 +797,7 @@
         <v>7</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -833,25 +841,31 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{4B698EE0-7D88-492A-BCD0-030ADC8D4978}"/>
     <hyperlink ref="B4" r:id="rId2" xr:uid="{6176ED7E-12C9-4014-A2AD-7F06CFA5C3D6}"/>
-    <hyperlink ref="B11" r:id="rId3" xr:uid="{68BAA6E3-83A8-4BF9-8591-76A52CC3C3BE}"/>
-    <hyperlink ref="B18" r:id="rId4" xr:uid="{344CDE2B-B701-4971-9A33-8540C0102698}"/>
+    <hyperlink ref="B12" r:id="rId3" xr:uid="{68BAA6E3-83A8-4BF9-8591-76A52CC3C3BE}"/>
+    <hyperlink ref="B19" r:id="rId4" xr:uid="{344CDE2B-B701-4971-9A33-8540C0102698}"/>
     <hyperlink ref="B22" r:id="rId5" xr:uid="{17ACA873-EA8C-4D49-BC23-0E03EBEF1A66}"/>
     <hyperlink ref="B23" r:id="rId6" xr:uid="{99C031E5-19BF-4A46-B281-5CF5A08DB3E5}"/>
     <hyperlink ref="B25" r:id="rId7" xr:uid="{2BE8A6BF-B94C-479C-B479-89F4364EB16B}"/>
-    <hyperlink ref="B26" r:id="rId8" xr:uid="{DB609696-5CDD-43E9-B09E-82D9C256E61C}"/>
-    <hyperlink ref="B27" r:id="rId9" xr:uid="{6904E5B6-BC47-4DE3-9399-FB7460432B60}"/>
-    <hyperlink ref="B29" r:id="rId10" xr:uid="{C0D025B4-CA17-4224-BB3F-C73ECBDFCA7C}"/>
-    <hyperlink ref="B32" r:id="rId11" xr:uid="{A47BA1E5-2B8A-4818-8E24-9848D29625C2}"/>
-    <hyperlink ref="B33" r:id="rId12" xr:uid="{2395E32C-D1F9-424B-AE5D-079F40DEA222}"/>
-    <hyperlink ref="B34" r:id="rId13" xr:uid="{60414CA4-4CEA-4C88-8F88-8DE99C190232}"/>
-    <hyperlink ref="B36" r:id="rId14" xr:uid="{BF57AEDF-0569-4878-82D9-819D529A96F9}"/>
-    <hyperlink ref="B38" r:id="rId15" xr:uid="{32B9AE79-2C60-4F53-94DC-E39B6D105A16}"/>
-    <hyperlink ref="B39" r:id="rId16" xr:uid="{B5DB55AC-9A89-40E4-8830-3A0CFE137486}"/>
-    <hyperlink ref="B35" r:id="rId17" xr:uid="{6D0240EE-4619-4357-8BC9-904568F0C456}"/>
-    <hyperlink ref="B14" r:id="rId18" xr:uid="{24CDB8D1-6919-447E-99AE-59DCA36AF49E}"/>
-    <hyperlink ref="B17" r:id="rId19" xr:uid="{0C57FDF8-4D29-4DF4-911D-EE27EEAECD05}"/>
+    <hyperlink ref="B27" r:id="rId8" xr:uid="{6904E5B6-BC47-4DE3-9399-FB7460432B60}"/>
+    <hyperlink ref="B29" r:id="rId9" xr:uid="{C0D025B4-CA17-4224-BB3F-C73ECBDFCA7C}"/>
+    <hyperlink ref="B32" r:id="rId10" xr:uid="{A47BA1E5-2B8A-4818-8E24-9848D29625C2}"/>
+    <hyperlink ref="B33" r:id="rId11" xr:uid="{2395E32C-D1F9-424B-AE5D-079F40DEA222}"/>
+    <hyperlink ref="B34" r:id="rId12" xr:uid="{60414CA4-4CEA-4C88-8F88-8DE99C190232}"/>
+    <hyperlink ref="B36" r:id="rId13" xr:uid="{BF57AEDF-0569-4878-82D9-819D529A96F9}"/>
+    <hyperlink ref="B38" r:id="rId14" xr:uid="{32B9AE79-2C60-4F53-94DC-E39B6D105A16}"/>
+    <hyperlink ref="B39" r:id="rId15" xr:uid="{B5DB55AC-9A89-40E4-8830-3A0CFE137486}"/>
+    <hyperlink ref="B35" r:id="rId16" xr:uid="{6D0240EE-4619-4357-8BC9-904568F0C456}"/>
+    <hyperlink ref="B15" r:id="rId17" xr:uid="{24CDB8D1-6919-447E-99AE-59DCA36AF49E}"/>
+    <hyperlink ref="B18" r:id="rId18" xr:uid="{0C57FDF8-4D29-4DF4-911D-EE27EEAECD05}"/>
+    <hyperlink ref="B5" r:id="rId19" xr:uid="{2708D437-96BC-4A08-B8BA-C8A7556BCE52}"/>
+    <hyperlink ref="B20" r:id="rId20" xr:uid="{A530AD06-F6EF-4FE8-9AE9-AFA5EDFD8D54}"/>
+    <hyperlink ref="B9" r:id="rId21" xr:uid="{01F0F796-63FF-4D61-94B2-1324FB119159}"/>
+    <hyperlink ref="B11" r:id="rId22" xr:uid="{4B17F157-3DC6-4057-BD4D-211E5DD0663A}"/>
+    <hyperlink ref="B13" r:id="rId23" xr:uid="{F8FD7C7A-0E9F-4982-A62D-6579AF75EB10}"/>
+    <hyperlink ref="B26" r:id="rId24" xr:uid="{19E8E3E0-231A-43CF-947F-02DABFD9F9B0}"/>
+    <hyperlink ref="B8" r:id="rId25" xr:uid="{88D7C21A-8A93-4786-AB7D-90A12BDF10B9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed bug. Openstaande bestelling/ PR's werden niet goed overgeschreven. Nu Wel
</commit_message>
<xml_diff>
--- a/Projectleiders.xlsx
+++ b/Projectleiders.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bram.gerrits\Desktop\Automations\ProjectAdministration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF681BF-A305-4A28-BCA1-EB4C057DBE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596FDE06-0629-438B-9DCD-0D0D3B1EE5FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
   <si>
     <t>Naam</t>
   </si>
@@ -523,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -641,9 +641,6 @@
       <c r="B13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D13" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -657,9 +654,6 @@
       <c r="B15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D15" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -782,7 +776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -790,7 +784,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -798,7 +792,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -809,33 +803,48 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>40</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>42</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D38" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>43</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="D39" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -870,8 +879,9 @@
     <hyperlink ref="B13" r:id="rId23" xr:uid="{F8FD7C7A-0E9F-4982-A62D-6579AF75EB10}"/>
     <hyperlink ref="B26" r:id="rId24" xr:uid="{19E8E3E0-231A-43CF-947F-02DABFD9F9B0}"/>
     <hyperlink ref="B8" r:id="rId25" xr:uid="{88D7C21A-8A93-4786-AB7D-90A12BDF10B9}"/>
+    <hyperlink ref="B37" r:id="rId26" xr:uid="{590523D9-160C-4876-863E-3CF72D237CAC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId27"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
made various changed concerning mail_for_closing to ask projectleaders if projects can be closed when certain conditions have been met
</commit_message>
<xml_diff>
--- a/Projectleiders.xlsx
+++ b/Projectleiders.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bram.gerrits\Desktop\Automations\ProjectAdministration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596FDE06-0629-438B-9DCD-0D0D3B1EE5FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D95AE4-6338-45ED-9CAA-30AFA5A20587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
   <si>
     <t>Naam</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>David.fontijn@vhe.nl</t>
+  </si>
+  <si>
+    <t>Maarten.lox@vhe.nl</t>
   </si>
 </sst>
 </file>
@@ -523,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -613,7 +616,12 @@
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -622,6 +630,9 @@
       <c r="B11" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -654,6 +665,9 @@
       <c r="B15" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -686,10 +700,13 @@
         <v>3</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -880,8 +897,9 @@
     <hyperlink ref="B26" r:id="rId24" xr:uid="{19E8E3E0-231A-43CF-947F-02DABFD9F9B0}"/>
     <hyperlink ref="B8" r:id="rId25" xr:uid="{88D7C21A-8A93-4786-AB7D-90A12BDF10B9}"/>
     <hyperlink ref="B37" r:id="rId26" xr:uid="{590523D9-160C-4876-863E-3CF72D237CAC}"/>
+    <hyperlink ref="B10" r:id="rId27" xr:uid="{D3C9510F-4BA9-4760-9831-017E217A2C8B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId27"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
moved to Finance map
</commit_message>
<xml_diff>
--- a/Projectleiders.xlsx
+++ b/Projectleiders.xlsx
@@ -495,7 +495,10 @@
         </is>
       </c>
       <c r="D2" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>45987</v>
       </c>
     </row>
     <row r="3">
@@ -535,7 +538,10 @@
         </is>
       </c>
       <c r="D5" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>45987</v>
       </c>
     </row>
     <row r="6">
@@ -550,7 +556,7 @@
         </is>
       </c>
       <c r="D6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -565,7 +571,10 @@
         </is>
       </c>
       <c r="D7" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>45987</v>
       </c>
     </row>
     <row r="8">
@@ -580,7 +589,7 @@
         </is>
       </c>
       <c r="D8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -595,7 +604,10 @@
         </is>
       </c>
       <c r="D9" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>45987</v>
       </c>
     </row>
     <row r="10">
@@ -625,7 +637,10 @@
         </is>
       </c>
       <c r="D11" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>45987</v>
       </c>
     </row>
     <row r="12">
@@ -655,7 +670,10 @@
         </is>
       </c>
       <c r="D13" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>45987</v>
       </c>
     </row>
     <row r="14">
@@ -905,7 +923,10 @@
         </is>
       </c>
       <c r="D32" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>45987</v>
       </c>
     </row>
     <row r="33">
@@ -920,7 +941,7 @@
         </is>
       </c>
       <c r="D33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -935,7 +956,7 @@
         </is>
       </c>
       <c r="D34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -958,7 +979,7 @@
         <v>1</v>
       </c>
       <c r="E35" s="2" t="n">
-        <v>45980</v>
+        <v>45987</v>
       </c>
     </row>
     <row r="36">
@@ -973,7 +994,7 @@
         </is>
       </c>
       <c r="D36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -988,7 +1009,10 @@
         </is>
       </c>
       <c r="D37" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>45987</v>
       </c>
     </row>
     <row r="38">
@@ -1003,7 +1027,7 @@
         </is>
       </c>
       <c r="D38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -1018,7 +1042,10 @@
         </is>
       </c>
       <c r="D39" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>45987</v>
       </c>
     </row>
   </sheetData>

</xml_diff>